<commit_message>
I changed the city to region
</commit_message>
<xml_diff>
--- a/Excel lab.xlsx
+++ b/Excel lab.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25683\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\25683\Desktop\git-workspace\Excel-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715A1E38-056F-40FA-825C-73D3DCE38DDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4334739-93ED-4A63-917F-B5F76210AD41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Salary" sheetId="1" r:id="rId1"/>
@@ -115,13 +115,13 @@
     <t>RANK</t>
   </si>
   <si>
-    <t>THE BEST CITY AND GENDER DISTRIBUTION OF IT JOBS</t>
-  </si>
-  <si>
     <t>Tatal Average</t>
   </si>
   <si>
     <t xml:space="preserve">IT Project Manager </t>
+  </si>
+  <si>
+    <t>THE BEST REGION AND GENDER DISTRIBUTION OF IT JOBS</t>
   </si>
 </sst>
 </file>
@@ -3474,10 +3474,10 @@
       <xdr:rowOff>106088</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>112449</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>43794</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>43793</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3492,8 +3492,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5155307" y="4346036"/>
-          <a:ext cx="3556100" cy="1858444"/>
+          <a:off x="5156448" y="4343071"/>
+          <a:ext cx="3996312" cy="2357274"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3576,7 +3576,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>he best city and gender</a:t>
+            <a:t>he best region</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>and gender</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
@@ -3612,7 +3636,21 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> in Canada. The best city in Canada for IT jobs is Toronto.</a:t>
+            <a:t> in Canada. </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The best city in Canada for IT jobs is Toronto.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3934,8 +3972,8 @@
   </sheetPr>
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4053,7 +4091,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="14">
         <v>52000</v>
@@ -4210,8 +4248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2935B96-C0AA-41F7-9BE6-6433C1B48D5E}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="58" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4223,7 +4261,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="39" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -4386,7 +4424,7 @@
     <row r="13" spans="1:4" ht="21.5" thickTop="1" x14ac:dyDescent="0.5">
       <c r="A13" s="37"/>
       <c r="B13" s="37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="36">
         <f>AVERAGE($C$3:$C$12)</f>

</xml_diff>